<commit_message>
Strip __S from sample name
</commit_message>
<xml_diff>
--- a/testdata/hdr/samplesheet.xlsx
+++ b/testdata/hdr/samplesheet.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olgabot/code/nf-core/nf-core-crisprvar/test-data/hdr/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847DCB7-7727-2149-A159-DBDDDFC6D73E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="24260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
+    <t>amplicon_seq</t>
+  </si>
+  <si>
+    <t>expected_hdr_amplicon_seq</t>
+  </si>
+  <si>
+    <t>guide_seq</t>
+  </si>
+  <si>
     <t>sample_id</t>
   </si>
   <si>
-    <t>amplicon_seq</t>
-  </si>
-  <si>
-    <t>expected_hdr_amplicon_seq</t>
-  </si>
-  <si>
-    <t>guide_seq</t>
-  </si>
-  <si>
     <t>CAAGAGCACGTCGCAGAAGCGCCCGCCGTTTTTGCGCTGCTGGTTCAGGTTGTGCAGCATCTCCGTGCTGTGTCTGCTCACCTGGTATGTGTAGCAGCCAGACGGGCCGCACGAAGCGTCGTTCACCCGCTCCATGGCCGCCGCCCCCTCCCACTAGCCCGGCCGCTGCACCTGCCCGCCCCCTCCCTTCCCCTCAGCAGCGAGAAGCGGGGCGCAGCAGACGTGTCCACACTCCCCACACGTGCCGGCCCGAGGCTCTGTAGTCTCG</t>
   </si>
   <si>
@@ -61,20 +55,20 @@
     <t>GGAGAAGAGGCTTATTCGGC</t>
   </si>
   <si>
-    <t>mNGplate11_sorted_A10_PATZ1-N__S9</t>
-  </si>
-  <si>
-    <t>mNGplate11_sorted_A11_KDELR3-C__S10</t>
-  </si>
-  <si>
-    <t>mNGplate11_sorted_A12_MYH9-C__S11</t>
+    <t>mNGplate11_sorted_A10_PATZ1-N</t>
+  </si>
+  <si>
+    <t>mNGplate11_sorted_A11_KDELR3-C</t>
+  </si>
+  <si>
+    <t>mNGplate11_sorted_A12_MYH9-C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,14 +131,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -191,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -223,27 +209,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,24 +243,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -468,30 +418,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -505,7 +453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -519,7 +467,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>

</xml_diff>